<commit_message>
generation of Gweru data.
</commit_message>
<xml_diff>
--- a/Project 1 -/Data_files/Cities/Gweru/Datafiles/Loan Given Report -  Gweru Mon 29 08 2022.xlsx
+++ b/Project 1 -/Data_files/Cities/Gweru/Datafiles/Loan Given Report -  Gweru Mon 29 08 2022.xlsx
@@ -1,28 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faith Kabanda\OneDrive\Documents\Data Analysis Portfolio By Faith Kabanda\Data-Analyst-Portfolio-By-Faith-Kabanda\Project 1 -\Data_files\Cities\Gweru\Datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7462868E-80F1-473C-AC96-4C70FE633565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579E49A4-36D3-4C2C-B554-AAA9CF2C16D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="826" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Loans given" sheetId="2" r:id="rId2"/>
     <sheet name="Loan given repayments" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -54,57 +64,18 @@
     <t>Citizenship</t>
   </si>
   <si>
-    <t>Odu Gloria</t>
-  </si>
-  <si>
-    <t>oduglo1@gmail.com</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
     <t>Married</t>
   </si>
   <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Idemudia Patience</t>
-  </si>
-  <si>
-    <t>patienceidemudia08@gmail.com</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
-    <t>Ezeh Degreat</t>
-  </si>
-  <si>
-    <t>ezehjohn902@gmail.com</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Prince Nnanna</t>
-  </si>
-  <si>
-    <t>princennemek5@gmail.com</t>
-  </si>
-  <si>
-    <t>Bola Igbirease</t>
-  </si>
-  <si>
-    <t>bolaigbirease@gmail.com</t>
-  </si>
-  <si>
-    <t>Paschal Iyamu</t>
-  </si>
-  <si>
-    <t>paschaliyamu9@gmail.com</t>
-  </si>
-  <si>
     <t>Loan given data ID</t>
   </si>
   <si>
@@ -199,6 +170,69 @@
   </si>
   <si>
     <t>Loan given repayment report tag</t>
+  </si>
+  <si>
+    <t>129938</t>
+  </si>
+  <si>
+    <t>135128</t>
+  </si>
+  <si>
+    <t>135430</t>
+  </si>
+  <si>
+    <t>135525</t>
+  </si>
+  <si>
+    <t>161237</t>
+  </si>
+  <si>
+    <t>168729</t>
+  </si>
+  <si>
+    <t>City of Residence</t>
+  </si>
+  <si>
+    <t>Gweru</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Gloria</t>
+  </si>
+  <si>
+    <t>Patience</t>
+  </si>
+  <si>
+    <t>Degreat</t>
+  </si>
+  <si>
+    <t>Nnanna</t>
+  </si>
+  <si>
+    <t>Igbire</t>
+  </si>
+  <si>
+    <t>Iyamu</t>
+  </si>
+  <si>
+    <t>o1@xmail.com</t>
+  </si>
+  <si>
+    <t>pa08@xmail.com</t>
+  </si>
+  <si>
+    <t>e2@xmail.com</t>
+  </si>
+  <si>
+    <t>p5@xmail.com</t>
+  </si>
+  <si>
+    <t>be@xmail.com</t>
+  </si>
+  <si>
+    <t>pas@xmail.com</t>
   </si>
 </sst>
 </file>
@@ -585,11 +619,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,24 +651,24 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1299</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>38</v>
@@ -641,27 +677,27 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1351</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>28</v>
@@ -670,27 +706,27 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1354</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -699,27 +735,27 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1355</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>25</v>
@@ -728,27 +764,27 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1612</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>37</v>
@@ -757,27 +793,27 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1687</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
       </c>
       <c r="F7">
         <v>29</v>
@@ -786,13 +822,13 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -806,9 +842,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,61 +876,61 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -908,9 +944,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,43 +978,43 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>